<commit_message>
Introduction to Monte Carlo
</commit_message>
<xml_diff>
--- a/Probalistic Loan IRR.xlsx
+++ b/Probalistic Loan IRR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marconunez/Documents/Financial Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE48576E-D188-7B45-9DFF-0A97DF2B258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB790A6D-BFB6-C044-B41A-C4D3B54CC830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{F006A279-74DE-4730-BD3F-EC878179084F}"/>
+    <workbookView xWindow="17440" yWindow="740" windowWidth="12800" windowHeight="18900" xr2:uid="{F006A279-74DE-4730-BD3F-EC878179084F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs and Outputs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Inputs</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Cash Flows</t>
   </si>
   <si>
     <t>=Outputs when using Excel for a single default case at once</t>
@@ -115,9 +112,6 @@
     <t>Recovery</t>
   </si>
   <si>
-    <t>Base Payment</t>
-  </si>
-  <si>
     <t>Recovery helper</t>
   </si>
   <si>
@@ -125,6 +119,15 @@
   </si>
   <si>
     <t>Payments</t>
+  </si>
+  <si>
+    <t>Recovery Payment</t>
+  </si>
+  <si>
+    <t>irr</t>
+  </si>
+  <si>
+    <t>Final Payment</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -372,7 +375,6 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +417,9 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -733,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0EC6A6-1631-4011-AD0B-8BE8683B88BB}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -744,10 +749,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -758,7 +763,7 @@
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -768,9 +773,12 @@
       <c r="B3" s="17">
         <v>20</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="45">
+        <f ca="1">IRR('Cash Flow'!K13:'Cash Flow'!K35)</f>
+        <v>0.34092110302163725</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -822,70 +830,68 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="34"/>
+      <c r="A14" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="33"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="D14" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="30" t="s">
+      <c r="E15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="31" t="s">
-        <v>14</v>
+      <c r="G15" s="30" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="12"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="21"/>
       <c r="B17" s="12"/>
       <c r="C17" s="3"/>
       <c r="D17" s="15">
@@ -897,7 +903,9 @@
       <c r="F17" s="6">
         <v>0.1</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="25">
+        <v>0.15149575271280002</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -914,7 +922,9 @@
       <c r="F18" s="6">
         <v>0.2</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="25">
+        <v>5.9631650559442216E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
@@ -931,7 +941,9 @@
       <c r="F19" s="6">
         <v>0.3</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="G19" s="25">
+        <v>-2.7632107591892465E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -948,7 +960,9 @@
       <c r="F20" s="6">
         <v>0.1</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="25">
+        <v>0.19131688454631779</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
@@ -965,7 +979,9 @@
       <c r="F21" s="6">
         <v>0.2</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="25">
+        <v>6.4163798883459938E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
@@ -982,7 +998,9 @@
       <c r="F22" s="6">
         <v>0.3</v>
       </c>
-      <c r="G22" s="26"/>
+      <c r="G22" s="25">
+        <v>-3.7549903600861603E-3</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
@@ -999,7 +1017,9 @@
       <c r="F23" s="6">
         <v>0.1</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="25">
+        <v>0.18319433223875983</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
@@ -1016,7 +1036,9 @@
       <c r="F24" s="6">
         <v>0.2</v>
       </c>
-      <c r="G24" s="26"/>
+      <c r="G24" s="25">
+        <v>6.544053598634289E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
@@ -1033,7 +1055,9 @@
       <c r="F25" s="6">
         <v>0.3</v>
       </c>
-      <c r="G25" s="26"/>
+      <c r="G25" s="25">
+        <v>8.2238203040650455E-3</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -1050,7 +1074,9 @@
       <c r="F26" s="6">
         <v>0.1</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="25">
+        <v>0.18561518479797848</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1068,7 +1094,9 @@
       <c r="F27" s="6">
         <v>0.2</v>
       </c>
-      <c r="G27" s="26"/>
+      <c r="G27" s="25">
+        <v>0.1420783232110161</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
@@ -1085,7 +1113,9 @@
       <c r="F28" s="6">
         <v>0.3</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="25">
+        <v>2.8037304928115306E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
@@ -1102,7 +1132,9 @@
       <c r="F29" s="6">
         <v>0.1</v>
       </c>
-      <c r="G29" s="26"/>
+      <c r="G29" s="25">
+        <v>0.2299370676165067</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
@@ -1119,7 +1151,9 @@
       <c r="F30" s="6">
         <v>0.2</v>
       </c>
-      <c r="G30" s="26"/>
+      <c r="G30" s="25">
+        <v>0.12653851051308815</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
@@ -1136,7 +1170,9 @@
       <c r="F31" s="6">
         <v>0.3</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="25">
+        <v>-4.4893515984652521E-3</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
@@ -1153,7 +1189,9 @@
       <c r="F32" s="6">
         <v>0.1</v>
       </c>
-      <c r="G32" s="26"/>
+      <c r="G32" s="25">
+        <v>0.18279319921047701</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
@@ -1170,7 +1208,9 @@
       <c r="F33" s="6">
         <v>0.2</v>
       </c>
-      <c r="G33" s="26"/>
+      <c r="G33" s="25">
+        <v>0.11790719885424419</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
@@ -1187,7 +1227,9 @@
       <c r="F34" s="6">
         <v>0.3</v>
       </c>
-      <c r="G34" s="26"/>
+      <c r="G34" s="25">
+        <v>-5.1424577042087404E-3</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
@@ -1204,7 +1246,9 @@
       <c r="F35" s="6">
         <v>0.1</v>
       </c>
-      <c r="G35" s="26"/>
+      <c r="G35" s="25">
+        <v>0.22905894642969543</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
@@ -1221,7 +1265,9 @@
       <c r="F36" s="6">
         <v>0.2</v>
       </c>
-      <c r="G36" s="26"/>
+      <c r="G36" s="25">
+        <v>0.10353463943338777</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
@@ -1238,7 +1284,9 @@
       <c r="F37" s="6">
         <v>0.3</v>
       </c>
-      <c r="G37" s="26"/>
+      <c r="G37" s="25">
+        <v>6.4655696998393568E-5</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
@@ -1255,7 +1303,9 @@
       <c r="F38" s="6">
         <v>0.1</v>
       </c>
-      <c r="G38" s="26"/>
+      <c r="G38" s="25">
+        <v>0.25183133582436645</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
@@ -1272,7 +1322,9 @@
       <c r="F39" s="6">
         <v>0.2</v>
       </c>
-      <c r="G39" s="26"/>
+      <c r="G39" s="25">
+        <v>0.15439693442852931</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
@@ -1289,7 +1341,9 @@
       <c r="F40" s="6">
         <v>0.3</v>
       </c>
-      <c r="G40" s="26"/>
+      <c r="G40" s="25">
+        <v>5.815026188164911E-2</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="14">
@@ -1306,7 +1360,9 @@
       <c r="F41" s="6">
         <v>0.1</v>
       </c>
-      <c r="G41" s="26"/>
+      <c r="G41" s="25">
+        <v>0.27791995375346146</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
@@ -1321,7 +1377,9 @@
       <c r="F42" s="6">
         <v>0.2</v>
       </c>
-      <c r="G42" s="26"/>
+      <c r="G42" s="25">
+        <v>0.14042225007923814</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
@@ -1336,7 +1394,9 @@
       <c r="F43" s="10">
         <v>0.3</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="26">
+        <v>4.3446520671214101E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1349,6 +1409,18 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D14:G14"/>
   </mergeCells>
+  <conditionalFormatting sqref="G17:G43">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1359,7 +1431,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1372,17 +1444,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="38"/>
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Inputs and Outputs'!A2</f>
         <v>Price of Machine</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="39">
         <f>'Inputs and Outputs'!B2</f>
         <v>1000000</v>
       </c>
@@ -1393,6 +1465,7 @@
         <v>Loan Life</v>
       </c>
       <c r="B3">
+        <f>'Inputs and Outputs'!B3</f>
         <v>20</v>
       </c>
     </row>
@@ -1401,8 +1474,9 @@
         <f>'Inputs and Outputs'!A4</f>
         <v>Initial Default Probability</v>
       </c>
-      <c r="B4" s="39">
-        <v>0.2</v>
+      <c r="B4" s="38">
+        <f>'Inputs and Outputs'!B4</f>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,7 +1484,7 @@
         <f>'Inputs and Outputs'!A5</f>
         <v>Decay of Default Probability</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="38">
         <f>'Inputs and Outputs'!B5</f>
         <v>0.9</v>
       </c>
@@ -1420,23 +1494,23 @@
         <f>'Inputs and Outputs'!A6</f>
         <v>Final Default Probability</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="38">
         <f>'Inputs and Outputs'!B6</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1453,7 +1527,7 @@
       </c>
       <c r="D14" s="1">
         <f>B4</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,7 +1544,7 @@
       </c>
       <c r="D15" s="1">
         <f>IF(C15&lt;1,D14*$B$5,IF(C15=1,$B$6,0))</f>
-        <v>0.18000000000000002</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1487,7 +1561,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ref="D16:D33" si="1">IF(C16&lt;1,D15*$B$5,IF(C16=1,$B$6,0))</f>
-        <v>0.16200000000000003</v>
+        <v>0.24300000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1504,7 +1578,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>0.14580000000000004</v>
+        <v>0.21870000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1521,7 +1595,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>0.13122000000000003</v>
+        <v>0.19683000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1538,7 +1612,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>0.11809800000000004</v>
+        <v>0.17714700000000003</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1555,7 +1629,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>0.10628820000000004</v>
+        <v>0.15943230000000003</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1572,7 +1646,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>9.5659380000000044E-2</v>
+        <v>0.14348907000000002</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1589,7 +1663,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>8.6093442000000048E-2</v>
+        <v>0.12914016300000003</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1606,14 +1680,14 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>7.748409780000004E-2</v>
-      </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
+        <v>0.11622614670000003</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1629,7 +1703,7 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
-        <v>6.9735688020000033E-2</v>
+        <v>0.10460353203000003</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1646,7 +1720,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>6.2762119218000026E-2</v>
+        <v>9.4143178827000032E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1663,7 +1737,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>5.6485907296200025E-2</v>
+        <v>8.472886094430003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1680,7 +1754,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>5.0837316566580026E-2</v>
+        <v>7.6255974849870026E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1697,7 +1771,7 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" si="1"/>
-        <v>4.5753584909922027E-2</v>
+        <v>6.8630377364883019E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1714,7 +1788,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>4.1178226418929827E-2</v>
+        <v>6.1767339628394716E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1731,7 +1805,7 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" si="1"/>
-        <v>3.7060403777036843E-2</v>
+        <v>5.5590605665555244E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1748,7 +1822,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" si="1"/>
-        <v>3.3354363399333162E-2</v>
+        <v>5.0031545098999722E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1765,12 +1839,12 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" si="1"/>
-        <v>3.0018927059399847E-2</v>
-      </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
+        <v>4.502839058909975E-2</v>
+      </c>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1799,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128DD78C-3C63-6445-8A2C-9EF3696233E8}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1814,26 +1888,28 @@
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'P default'!A2</f>
         <v>Price of Machine</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="39">
         <f>'P default'!B2</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'P default'!A3</f>
         <v>Loan Life</v>
@@ -1843,27 +1919,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'Inputs and Outputs'!A7</f>
         <v>Recovery Rate</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="38">
         <f>'Inputs and Outputs'!B7</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="str">
         <f>'Inputs and Outputs'!A8</f>
         <v>Interest Rate</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="38">
         <f>'Inputs and Outputs'!B8</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Inputs and Outputs'!A9</f>
         <v>Default Year</v>
@@ -1873,60 +1949,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="43">
-        <f>B2/B3</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="42"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="str">
         <f>'P default'!D13</f>
         <v>Defaul Probability</v>
       </c>
       <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="J12" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
         <v>29</v>
       </c>
-      <c r="I12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="1">
-        <f>IRR(H13:H35)</f>
-        <v>0.35784967093146314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
-      <c r="B13" s="39">
-        <v>0</v>
-      </c>
-      <c r="C13" s="39">
+      <c r="B13" s="38">
+        <v>0</v>
+      </c>
+      <c r="C13" s="38">
         <v>0</v>
       </c>
       <c r="D13">
@@ -1943,30 +2015,37 @@
         <f>SUM($F$13:F13)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="43">
+      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="I13" s="39">
+        <v>0</v>
+      </c>
+      <c r="J13" s="39">
+        <f>IF(AND(A13=$B$3, E13=0), $B$2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="42">
         <f>-B2</f>
         <v>-1000000</v>
       </c>
-      <c r="I13" s="43">
-        <f>-B2</f>
-        <v>-1000000</v>
-      </c>
-      <c r="J13" s="1">
-        <f ca="1">IRR(I13:I35)</f>
-        <v>-0.70924635468163366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="43">
+        <f ca="1">IRR(K13:K35)</f>
+        <v>0.34092110302163725</v>
+      </c>
+      <c r="N13" s="44"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="38">
         <f>'P default'!D14</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C14">
         <f ca="1">RAND()</f>
-        <v>0.90971921743475226</v>
+        <v>0.30240051292803316</v>
       </c>
       <c r="D14">
         <f ca="1">IF(C14&lt;B14, 1, 0)</f>
@@ -1983,30 +2062,38 @@
         <f>SUM($F$13:F14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="43">
-        <f>B7</f>
-        <v>50000</v>
-      </c>
-      <c r="I14" s="43">
-        <f ca="1">IF(D14=0, B7, 0)</f>
-        <v>50000</v>
-      </c>
-      <c r="J14" s="43"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="42">
+        <f ca="1">IF(AND(D14=1,E14=1),0,$B$2*$B$5)</f>
+        <v>400000</v>
+      </c>
+      <c r="I14" s="39">
+        <f>IF(AND(F14=1, G14=1), $B$4*$B$2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="39">
+        <f t="shared" ref="J14:J35" ca="1" si="0">IF(AND(A14=$B$3, E14=0), $B$2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="42">
+        <f ca="1">H14+I14+J14</f>
+        <v>400000</v>
+      </c>
+      <c r="L14" s="42"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="38">
         <f>'P default'!D15</f>
-        <v>0.18000000000000002</v>
+        <v>0.27</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C35" ca="1" si="0">RAND()</f>
-        <v>0.87238130245899137</v>
+        <f t="shared" ref="C15:C35" ca="1" si="1">RAND()</f>
+        <v>0.90057790320853348</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D35" ca="1" si="1">IF(C15&lt;B15, 1, 0)</f>
+        <f t="shared" ref="D15:D35" ca="1" si="2">IF(C15&lt;B15, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="E15">
@@ -2020,29 +2107,38 @@
         <f>SUM($F$13:F15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="43">
-        <f>H14*(1+$B$5)</f>
-        <v>70000</v>
-      </c>
-      <c r="I15" s="43">
-        <f ca="1">IF(D15=0,I14 *(1+$B$5), 0)</f>
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="42">
+        <f ca="1">IF(OR(A15&gt;$B$3, OR(D15=1, E15&gt;0)), 0, $B$2*$B$5)</f>
+        <v>400000</v>
+      </c>
+      <c r="I15" s="39">
+        <f t="shared" ref="I15:K35" si="3">IF(AND(F15=1, G15=1), $B$4*$B$2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="42">
+        <f t="shared" ref="K15:K35" ca="1" si="4">H15+I15+J15</f>
+        <v>400000</v>
+      </c>
+      <c r="L15" s="42"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="38">
         <f>'P default'!D16</f>
-        <v>0.16200000000000003</v>
+        <v>0.24300000000000002</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73495146317433713</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55806742983226665</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -2057,29 +2153,38 @@
         <f ca="1">SUM($F$13:F16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="43">
-        <f t="shared" ref="H16:H35" si="2">H15*(1+$B$5)</f>
-        <v>98000</v>
-      </c>
-      <c r="I16" s="43">
-        <f ca="1">IF(E16&lt;2, IF(F16=1, 0, 0), IF(AND(F16=1, G16&lt;2), $B$7 * $B$4, I15 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="42">
+        <f t="shared" ref="H16:H35" ca="1" si="5">IF(OR(A16&gt;$B$3, OR(D16=1, E16&gt;0)), 0, $B$2*$B$5)</f>
+        <v>400000</v>
+      </c>
+      <c r="I16" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>400000</v>
+      </c>
+      <c r="L16" s="42"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17" s="39">
+      <c r="B17" s="38">
         <f>'P default'!D17</f>
-        <v>0.14580000000000004</v>
+        <v>0.21870000000000003</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7977067745904598</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90510375864870385</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -2094,29 +2199,38 @@
         <f ca="1">SUM($F$13:F17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="43">
-        <f t="shared" si="2"/>
-        <v>137200</v>
-      </c>
-      <c r="I17" s="43">
-        <f ca="1">IF(E17&lt;2, IF(F17=1, 0, 0), IF(AND(F17=1, G17&lt;2), $B$7 * $B$4, I16 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>400000</v>
+      </c>
+      <c r="I17" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>400000</v>
+      </c>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
-      <c r="B18" s="39">
+      <c r="B18" s="38">
         <f>'P default'!D18</f>
-        <v>0.13122000000000003</v>
+        <v>0.19683000000000003</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.51366347770463638</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92111471863798566</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -2131,29 +2245,38 @@
         <f ca="1">SUM($F$13:F18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="43">
-        <f t="shared" si="2"/>
-        <v>192080</v>
-      </c>
-      <c r="I18" s="43">
-        <f ca="1">IF(E18&lt;2, IF(F18=1, 0, 0), IF(AND(F18=1, G18&lt;2), $B$7 * $B$4, I17 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>400000</v>
+      </c>
+      <c r="I18" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>400000</v>
+      </c>
+      <c r="L18" s="42"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
-      <c r="B19" s="39">
+      <c r="B19" s="38">
         <f>'P default'!D19</f>
-        <v>0.11809800000000004</v>
+        <v>0.17714700000000003</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.37983310253141411</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98601532873799413</v>
       </c>
       <c r="D19">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E19">
@@ -2168,29 +2291,38 @@
         <f ca="1">SUM($F$13:F19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="43">
-        <f t="shared" si="2"/>
-        <v>268912</v>
-      </c>
-      <c r="I19" s="43">
-        <f ca="1">IF(E19&lt;2, IF(F19=1, 0, 0), IF(AND(F19=1, G19&lt;2), $B$7 * $B$4, I18 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H19" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>400000</v>
+      </c>
+      <c r="I19" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>400000</v>
+      </c>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
-      <c r="B20" s="39">
+      <c r="B20" s="38">
         <f>'P default'!D20</f>
-        <v>0.10628820000000004</v>
+        <v>0.15943230000000003</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.2099014740208864E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>7.0604866589889403E-2</v>
       </c>
       <c r="D20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E20">
@@ -2205,29 +2337,38 @@
         <f ca="1">SUM($F$13:F20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="43">
-        <f t="shared" si="2"/>
-        <v>376476.8</v>
-      </c>
-      <c r="I20" s="43">
-        <f ca="1">IF(E20&lt;2, IF(F20=1, 0, 0), IF(AND(F20=1, G20&lt;2), $B$7 * $B$4, I19 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H20" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="42"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
-      <c r="B21" s="39">
+      <c r="B21" s="38">
         <f>'P default'!D21</f>
-        <v>9.5659380000000044E-2</v>
+        <v>0.14348907000000002</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.89649555439045303</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93104621267988386</v>
       </c>
       <c r="D21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E21">
@@ -2242,29 +2383,38 @@
         <f ca="1">SUM($F$13:F21)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="43">
-        <f t="shared" si="2"/>
-        <v>527067.5199999999</v>
-      </c>
-      <c r="I21" s="43">
-        <f ca="1">IF(E21&lt;2, IF(F21=1, 0, 0), IF(AND(F21=1, G21&lt;2), $B$7 * $B$4, I20 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H21" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="42"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
-      <c r="B22" s="39">
+      <c r="B22" s="38">
         <f>'P default'!D22</f>
-        <v>8.6093442000000048E-2</v>
+        <v>0.12914016300000003</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.54429354615791492</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7133372968118985</v>
       </c>
       <c r="D22">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E22">
@@ -2279,29 +2429,38 @@
         <f ca="1">SUM($F$13:F22)</f>
         <v>1</v>
       </c>
-      <c r="H22" s="43">
-        <f t="shared" si="2"/>
-        <v>737894.52799999982</v>
-      </c>
-      <c r="I22" s="43">
-        <f ca="1">IF(E22&lt;2, IF(F22=1, 0, 0), IF(AND(F22=1, G22&lt;2), $B$7 * $B$4, I21 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H22" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>400000</v>
+      </c>
+      <c r="J22" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>400000</v>
+      </c>
+      <c r="L22" s="42"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
-      <c r="B23" s="39">
+      <c r="B23" s="38">
         <f>'P default'!D23</f>
-        <v>7.748409780000004E-2</v>
+        <v>0.11622614670000003</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.3595268783006604E-3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.3232335627770198E-2</v>
       </c>
       <c r="D23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E23">
@@ -2316,29 +2475,38 @@
         <f ca="1">SUM($F$13:F23)</f>
         <v>1</v>
       </c>
-      <c r="H23" s="43">
-        <f t="shared" si="2"/>
-        <v>1033052.3391999997</v>
-      </c>
-      <c r="I23" s="43">
-        <f ca="1">IF(E23&lt;2, IF(F23=1, 0, 0), IF(AND(F23=1, G23&lt;2), $B$7 * $B$4, I22 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H23" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="42"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="38">
         <f>'P default'!D24</f>
-        <v>6.9735688020000033E-2</v>
+        <v>0.10460353203000003</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.52504807882841742</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31131335408469707</v>
       </c>
       <c r="D24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E24">
@@ -2353,29 +2521,38 @@
         <f ca="1">SUM($F$13:F24)</f>
         <v>1</v>
       </c>
-      <c r="H24" s="43">
-        <f t="shared" si="2"/>
-        <v>1446273.2748799995</v>
-      </c>
-      <c r="I24" s="43">
-        <f ca="1">IF(E24&lt;2, IF(F24=1, 0, 0), IF(AND(F24=1, G24&lt;2), $B$7 * $B$4, I23 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
-      <c r="B25" s="39">
+      <c r="B25" s="38">
         <f>'P default'!D25</f>
-        <v>6.2762119218000026E-2</v>
+        <v>9.4143178827000032E-2</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.99428016851474144</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68920904853285569</v>
       </c>
       <c r="D25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E25">
@@ -2390,29 +2567,38 @@
         <f ca="1">SUM($F$13:F25)</f>
         <v>2</v>
       </c>
-      <c r="H25" s="43">
-        <f t="shared" si="2"/>
-        <v>2024782.5848319991</v>
-      </c>
-      <c r="I25" s="43">
-        <f ca="1">IF(E25&lt;2, IF(F25=1, 0, 0), IF(AND(F25=1, G25&lt;2), $B$7 * $B$4, I24 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H25" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
-      <c r="B26" s="39">
+      <c r="B26" s="38">
         <f>'P default'!D26</f>
-        <v>5.6485907296200025E-2</v>
+        <v>8.472886094430003E-2</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.53654962387707528</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.24172718151777439</v>
       </c>
       <c r="D26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E26">
@@ -2427,29 +2613,38 @@
         <f ca="1">SUM($F$13:F26)</f>
         <v>2</v>
       </c>
-      <c r="H26" s="43">
-        <f t="shared" si="2"/>
-        <v>2834695.6187647986</v>
-      </c>
-      <c r="I26" s="43">
-        <f ca="1">IF(E26&lt;2, IF(F26=1, 0, 0), IF(AND(F26=1, G26&lt;2), $B$7 * $B$4, I25 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H26" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="39"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>14</v>
       </c>
-      <c r="B27" s="39">
+      <c r="B27" s="38">
         <f>'P default'!D27</f>
-        <v>5.0837316566580026E-2</v>
+        <v>7.6255974849870026E-2</v>
       </c>
       <c r="C27">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.47525299346346939</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15446350663223529</v>
       </c>
       <c r="D27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E27">
@@ -2464,29 +2659,38 @@
         <f ca="1">SUM($F$13:F27)</f>
         <v>2</v>
       </c>
-      <c r="H27" s="43">
-        <f t="shared" si="2"/>
-        <v>3968573.8662707177</v>
-      </c>
-      <c r="I27" s="43">
-        <f ca="1">IF(E27&lt;2, IF(F27=1, 0, 0), IF(AND(F27=1, G27&lt;2), $B$7 * $B$4, I26 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H27" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="39"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>15</v>
       </c>
-      <c r="B28" s="39">
+      <c r="B28" s="38">
         <f>'P default'!D28</f>
-        <v>4.5753584909922027E-2</v>
+        <v>6.8630377364883019E-2</v>
       </c>
       <c r="C28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1017594484156733</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10559516967133931</v>
       </c>
       <c r="D28">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E28">
@@ -2501,29 +2705,38 @@
         <f ca="1">SUM($F$13:F28)</f>
         <v>2</v>
       </c>
-      <c r="H28" s="43">
-        <f t="shared" si="2"/>
-        <v>5556003.4127790043</v>
-      </c>
-      <c r="I28" s="43">
-        <f ca="1">IF(E28&lt;2, IF(F28=1, 0, 0), IF(AND(F28=1, G28&lt;2), $B$7 * $B$4, I27 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H28" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="39"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>16</v>
       </c>
-      <c r="B29" s="39">
+      <c r="B29" s="38">
         <f>'P default'!D29</f>
-        <v>4.1178226418929827E-2</v>
+        <v>6.1767339628394716E-2</v>
       </c>
       <c r="C29">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28957246933952319</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36716667271042924</v>
       </c>
       <c r="D29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E29">
@@ -2538,29 +2751,38 @@
         <f ca="1">SUM($F$13:F29)</f>
         <v>2</v>
       </c>
-      <c r="H29" s="43">
-        <f t="shared" si="2"/>
-        <v>7778404.7778906059</v>
-      </c>
-      <c r="I29" s="43">
-        <f ca="1">IF(E29&lt;2, IF(F29=1, 0, 0), IF(AND(F29=1, G29&lt;2), $B$7 * $B$4, I28 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H29" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="39"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>17</v>
       </c>
-      <c r="B30" s="39">
+      <c r="B30" s="38">
         <f>'P default'!D30</f>
-        <v>3.7060403777036843E-2</v>
+        <v>5.5590605665555244E-2</v>
       </c>
       <c r="C30">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24128776331334689</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36886582571267224</v>
       </c>
       <c r="D30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E30">
@@ -2575,29 +2797,38 @@
         <f ca="1">SUM($F$13:F30)</f>
         <v>2</v>
       </c>
-      <c r="H30" s="43">
-        <f t="shared" si="2"/>
-        <v>10889766.689046847</v>
-      </c>
-      <c r="I30" s="43">
-        <f ca="1">IF(E30&lt;2, IF(F30=1, 0, 0), IF(AND(F30=1, G30&lt;2), $B$7 * $B$4, I29 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="39"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>18</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="38">
         <f>'P default'!D31</f>
-        <v>3.3354363399333162E-2</v>
+        <v>5.0031545098999722E-2</v>
       </c>
       <c r="C31">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.47141652083147267</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21712274787136154</v>
       </c>
       <c r="D31">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E31">
@@ -2612,29 +2843,38 @@
         <f ca="1">SUM($F$13:F31)</f>
         <v>2</v>
       </c>
-      <c r="H31" s="43">
-        <f t="shared" si="2"/>
-        <v>15245673.364665585</v>
-      </c>
-      <c r="I31" s="43">
-        <f ca="1">IF(E31&lt;2, IF(F31=1, 0, 0), IF(AND(F31=1, G31&lt;2), $B$7 * $B$4, I30 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H31" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="39"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>19</v>
       </c>
-      <c r="B32" s="39">
+      <c r="B32" s="38">
         <f>'P default'!D32</f>
-        <v>3.0018927059399847E-2</v>
+        <v>4.502839058909975E-2</v>
       </c>
       <c r="C32">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32595668734027283</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.72927134112114878</v>
       </c>
       <c r="D32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E32">
@@ -2649,29 +2889,38 @@
         <f ca="1">SUM($F$13:F32)</f>
         <v>2</v>
       </c>
-      <c r="H32" s="43">
-        <f t="shared" si="2"/>
-        <v>21343942.710531816</v>
-      </c>
-      <c r="I32" s="43">
-        <f ca="1">IF(E32&lt;2, IF(F32=1, 0, 0), IF(AND(F32=1, G32&lt;2), $B$7 * $B$4, I31 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
-      <c r="B33" s="39">
+      <c r="B33" s="38">
         <f>'P default'!D33</f>
         <v>0.4</v>
       </c>
       <c r="C33">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.52990162187380951</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.59471962447678706</v>
       </c>
       <c r="D33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E33">
@@ -2686,29 +2935,38 @@
         <f ca="1">SUM($F$13:F33)</f>
         <v>2</v>
       </c>
-      <c r="H33" s="43">
-        <f t="shared" si="2"/>
-        <v>29881519.79474454</v>
-      </c>
-      <c r="I33" s="43">
-        <f ca="1">IF(E33&lt;2, IF(F33=1, 0, 0), IF(AND(F33=1, G33&lt;2), $B$7 * $B$4, I32 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H33" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="39"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>21</v>
       </c>
-      <c r="B34" s="39">
+      <c r="B34" s="38">
         <f>'P default'!D34</f>
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.17652298847157566</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44605061723613315</v>
       </c>
       <c r="D34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E34">
@@ -2723,28 +2981,38 @@
         <f ca="1">SUM($F$13:F34)</f>
         <v>2</v>
       </c>
-      <c r="H34" s="43">
-        <v>0</v>
-      </c>
-      <c r="I34" s="43">
-        <f ca="1">IF(E34&lt;2, IF(F34=1, 0, 0), IF(AND(F34=1, G34&lt;2), $B$7 * $B$4, I33 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H34" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="39"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>22</v>
       </c>
-      <c r="B35" s="39">
+      <c r="B35" s="38">
         <f>'P default'!D35</f>
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.668033759831555</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23520888032258147</v>
       </c>
       <c r="D35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E35">
@@ -2759,13 +3027,23 @@
         <f ca="1">SUM($F$13:F35)</f>
         <v>2</v>
       </c>
-      <c r="H35" s="43">
-        <v>0</v>
-      </c>
-      <c r="I35" s="43">
-        <f ca="1">IF(E35&lt;2, IF(F35=1, 0, 0), IF(AND(F35=1, G35&lt;2), $B$7 * $B$4, I34 * (1 + $B$5)))</f>
-        <v>0</v>
-      </c>
+      <c r="H35" s="42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="42">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>